<commit_message>
train models and enable num_merge
</commit_message>
<xml_diff>
--- a/records/Summary.xlsx
+++ b/records/Summary.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jianq\Cochannel-Speech-Detector\records\Week 16\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cochannel-Speech-Detector1\records\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9428AF4-85B5-45BC-9C77-430194EE897F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB9BA17E-3FD5-4977-8353-B985F88EAF8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29580" yWindow="780" windowWidth="18900" windowHeight="11055" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 15" sheetId="2" r:id="rId1"/>
     <sheet name="Week 16" sheetId="1" r:id="rId2"/>
+    <sheet name="Week 17" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -454,7 +455,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FF51D1E-EAF0-4F43-A9D8-5371C7AF5A49}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -680,4 +681,16 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF4FAF4A-D831-4D2C-8799-663F1E4FA129}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>